<commit_message>
7.4 Добавлен rec_type with_post_recognition
</commit_message>
<xml_diff>
--- a/Lab7/Сводная таблица.xlsx
+++ b/Lab7/Сводная таблица.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>rec_type</t>
   </si>
@@ -37,19 +37,19 @@
     <t>wer</t>
   </si>
   <si>
-    <t>0.954</t>
-  </si>
-  <si>
     <t>val</t>
   </si>
   <si>
     <t>ds2</t>
   </si>
   <si>
-    <t>1.190</t>
-  </si>
-  <si>
     <t>augmented_recognition</t>
+  </si>
+  <si>
+    <t>with_post_recognition</t>
+  </si>
+  <si>
+    <t>classic teseract</t>
   </si>
 </sst>
 </file>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,127 +412,241 @@
     <col min="2" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>